<commit_message>
0 and 1 input solved,
</commit_message>
<xml_diff>
--- a/Excel/handover_data.xlsx
+++ b/Excel/handover_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>FormID</t>
   </si>
@@ -55,9 +55,6 @@
     <t>SenderRemarks</t>
   </si>
   <si>
-    <t>Reached</t>
-  </si>
-  <si>
     <t>ReceiverCondition</t>
   </si>
   <si>
@@ -79,43 +76,52 @@
     <t>Status</t>
   </si>
   <si>
-    <t>3cba214d</t>
+    <t>2ba1c34d</t>
+  </si>
+  <si>
+    <t>Drone Equipment</t>
+  </si>
+  <si>
+    <t>Name7</t>
+  </si>
+  <si>
+    <t>Make7</t>
+  </si>
+  <si>
+    <t>Model7</t>
+  </si>
+  <si>
+    <t>Serial7</t>
+  </si>
+  <si>
+    <t>SOI ASSAM</t>
+  </si>
+  <si>
+    <t>SOI TRIPURA</t>
+  </si>
+  <si>
+    <t>Umar</t>
+  </si>
+  <si>
+    <t>Not OK</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>Drone Equipment</t>
-  </si>
-  <si>
-    <t>Name7</t>
-  </si>
-  <si>
-    <t>Make7</t>
-  </si>
-  <si>
-    <t>Model7</t>
-  </si>
-  <si>
-    <t>Serial7</t>
-  </si>
-  <si>
-    <t>SOI ASSAM</t>
-  </si>
-  <si>
-    <t>Umar</t>
-  </si>
-  <si>
-    <t>Hammad</t>
-  </si>
-  <si>
-    <t>Not OK</t>
-  </si>
-  <si>
-    <t>2024-06-07 10:43:59</t>
-  </si>
-  <si>
-    <t>Pending</t>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>2024-06-07 12:54:38</t>
+  </si>
+  <si>
+    <t>2024-06-07 13:08:01</t>
+  </si>
+  <si>
+    <t>Rejected</t>
   </si>
 </sst>
 </file>
@@ -473,13 +479,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,70 +546,67 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>111111111111</v>
+      </c>
+      <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>27</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>28</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>28</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>30</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>31</v>
       </c>
-      <c r="N2" t="s">
-        <v>22</v>
-      </c>
       <c r="O2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="S2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T2" t="s">
-        <v>22</v>
-      </c>
-      <c r="U2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
transProg and transHist and pririty test left
</commit_message>
<xml_diff>
--- a/Excel/handover_data.xlsx
+++ b/Excel/handover_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
   <si>
     <t>FormID</t>
   </si>
@@ -79,37 +79,94 @@
     <t>2ba1c34d</t>
   </si>
   <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>sdsdsa</t>
+  </si>
+  <si>
+    <t>das</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>ca1bd423</t>
+  </si>
+  <si>
+    <t>aaaaaaaaaaaa</t>
+  </si>
+  <si>
+    <t>123412341234</t>
+  </si>
+  <si>
     <t>Drone Equipment</t>
   </si>
   <si>
+    <t>Electronics</t>
+  </si>
+  <si>
     <t>Name7</t>
   </si>
   <si>
+    <t>Name1</t>
+  </si>
+  <si>
     <t>Make7</t>
   </si>
   <si>
+    <t>Make1</t>
+  </si>
+  <si>
     <t>Model7</t>
   </si>
   <si>
+    <t>Model1</t>
+  </si>
+  <si>
     <t>Serial7</t>
   </si>
   <si>
+    <t>Serial1</t>
+  </si>
+  <si>
     <t>SOI ASSAM</t>
   </si>
   <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>ad</t>
+  </si>
+  <si>
     <t>SOI TRIPURA</t>
   </si>
   <si>
     <t>Umar</t>
   </si>
   <si>
+    <t>sdasd</t>
+  </si>
+  <si>
+    <t>Hammad</t>
+  </si>
+  <si>
+    <t>Fahad</t>
+  </si>
+  <si>
     <t>Not OK</t>
   </si>
   <si>
+    <t>Good</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
-    <t>Good</t>
+    <t>badhiya</t>
+  </si>
+  <si>
+    <t>Not Ok</t>
   </si>
   <si>
     <t>YES</t>
@@ -118,10 +175,16 @@
     <t>2024-06-07 12:54:38</t>
   </si>
   <si>
-    <t>2024-06-07 13:08:01</t>
-  </si>
-  <si>
-    <t>Rejected</t>
+    <t>2024-06-07 18:48:17</t>
+  </si>
+  <si>
+    <t>2024-06-07 19:25:29</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Approved</t>
   </si>
 </sst>
 </file>
@@ -479,7 +542,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -555,58 +618,335 @@
         <v>111111111111</v>
       </c>
       <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" t="s">
+        <v>52</v>
+      </c>
+      <c r="T2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B3">
+        <v>111111111111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B4">
+        <v>111111111111</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" t="s">
+        <v>48</v>
+      </c>
+      <c r="R4" t="s">
+        <v>52</v>
+      </c>
+      <c r="T4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5" t="s">
+        <v>48</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
+        <v>52</v>
+      </c>
+      <c r="S5" t="s">
+        <v>52</v>
+      </c>
+      <c r="T5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="B6">
+        <v>111111111111</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6" t="s">
+        <v>48</v>
+      </c>
+      <c r="R6" t="s">
+        <v>52</v>
+      </c>
+      <c r="S6" t="s">
+        <v>52</v>
+      </c>
+      <c r="T6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="J2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="C7" t="s">
         <v>29</v>
       </c>
-      <c r="M2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="D7" t="s">
         <v>31</v>
       </c>
-      <c r="O2" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="E7" t="s">
         <v>33</v>
       </c>
-      <c r="S2" t="s">
-        <v>34</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="F7" t="s">
         <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M7" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" t="s">
+        <v>50</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7" t="s">
+        <v>53</v>
+      </c>
+      <c r="S7" t="s">
+        <v>54</v>
+      </c>
+      <c r="T7" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eway bill Unique Constraints Added.
</commit_message>
<xml_diff>
--- a/Excel/handover_data.xlsx
+++ b/Excel/handover_data.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/12b12b08b9581f4a/Desktop/INS/IMS FINAL/Inventory-Management-System/Excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_2A0521E7F613C8264F2C4CE5C52EAD346DDE21B4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46595B68-5824-49BF-A3D6-F6743C06F29B}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t>FormID</t>
   </si>
@@ -79,6 +85,9 @@
     <t>a1d4b2c3</t>
   </si>
   <si>
+    <t>111111111111</t>
+  </si>
+  <si>
     <t>DGPS Equipment</t>
   </si>
   <si>
@@ -157,20 +166,20 @@
     <t>ap</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>2024-06-11 16:21:13</t>
   </si>
   <si>
-    <t>2024-06-11 16:25:57</t>
-  </si>
-  <si>
-    <t>Rejected</t>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +242,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -279,7 +296,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -311,9 +328,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -345,6 +380,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -520,14 +573,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="P2:Q5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -589,234 +644,239 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="B2">
-        <v>987654321123</v>
+      <c r="B2" t="s">
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
+        <v>46</v>
+      </c>
+      <c r="P2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>48</v>
       </c>
       <c r="R2" t="s">
-        <v>47</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="S2" t="s">
+        <v>48</v>
       </c>
       <c r="T2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3">
-        <v>987654321123</v>
+      <c r="B3" t="s">
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" t="s">
         <v>44</v>
       </c>
-      <c r="M3" t="s">
-        <v>46</v>
-      </c>
-      <c r="N3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
+      <c r="P3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>48</v>
       </c>
       <c r="R3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="S3" t="s">
         <v>48</v>
       </c>
       <c r="T3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4">
-        <v>987654321123</v>
+      <c r="B4" t="s">
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M4" t="s">
-        <v>45</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
+        <v>46</v>
+      </c>
+      <c r="P4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>48</v>
       </c>
       <c r="R4" t="s">
-        <v>47</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="S4" t="s">
+        <v>48</v>
       </c>
       <c r="T4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5">
-        <v>987654321123</v>
+      <c r="B5" t="s">
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N5" t="s">
-        <v>43</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="P5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>48</v>
       </c>
       <c r="R5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="S5" t="s">
         <v>48</v>
       </c>
       <c r="T5" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="S7" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>